<commit_message>
updated all bolt-on components to have FS of 1.5
</commit_message>
<xml_diff>
--- a/cc_mech_calcs.xlsx
+++ b/cc_mech_calcs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30200" yWindow="780" windowWidth="33240" windowHeight="18300" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="780" windowWidth="33240" windowHeight="18300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Proof Test Caps" sheetId="5" r:id="rId5"/>
     <sheet name="Butt Weld" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
   <si>
     <t>Component</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>Calculations competed utilizing Roark's Formulas for Stress &amp; Strain, Section 11.2</t>
+  </si>
+  <si>
+    <t>ta = tangential moment at the outer edge</t>
+  </si>
+  <si>
+    <t>rb = radial moment at the inner edge</t>
   </si>
 </sst>
 </file>
@@ -597,11 +603,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1404677232"/>
-        <c:axId val="-1402869952"/>
+        <c:axId val="313827488"/>
+        <c:axId val="313830240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1404677232"/>
+        <c:axId val="313827488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,12 +663,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1402869952"/>
+        <c:crossAx val="313830240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1402869952"/>
+        <c:axId val="313830240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1404677232"/>
+        <c:crossAx val="313827488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1624,7 +1630,7 @@
   <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1699,11 +1705,11 @@
       </c>
       <c r="F6">
         <f>'Injector Plate'!H3</f>
-        <v>0.5</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="G6">
         <f>'Injector Plate'!C16</f>
-        <v>1.7644110275689222</v>
+        <v>1.4997493734335841</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -1722,11 +1728,11 @@
       </c>
       <c r="F7">
         <f>'Aft Closeout'!H3</f>
-        <v>0.5</v>
+        <v>0.31</v>
       </c>
       <c r="G7">
         <f>'Aft Closeout'!C22</f>
-        <v>2.4318935186544914</v>
+        <v>1.5077739815657847</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
@@ -1756,6 +1762,16 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -2148,7 +2164,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2186,7 +2202,7 @@
         <v>7</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
@@ -2288,7 +2304,7 @@
       </c>
       <c r="C15">
         <f>6*C14/H3</f>
-        <v>18703.125</v>
+        <v>22003.676470588234</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -2300,7 +2316,7 @@
       </c>
       <c r="C16" s="2">
         <f>Overview!C21/'Injector Plate'!C15</f>
-        <v>1.7644110275689222</v>
+        <v>1.4997493734335841</v>
       </c>
     </row>
   </sheetData>
@@ -2313,7 +2329,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2351,7 +2367,7 @@
         <v>7</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.31</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
@@ -2513,7 +2529,7 @@
       </c>
       <c r="C21">
         <f>6*C20/H3</f>
-        <v>13569.673074443699</v>
+        <v>21886.569474909193</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
@@ -2525,7 +2541,7 @@
       </c>
       <c r="C22" s="2">
         <f>Overview!C21/'Aft Closeout'!C21</f>
-        <v>2.4318935186544914</v>
+        <v>1.5077739815657847</v>
       </c>
     </row>
   </sheetData>
@@ -2796,7 +2812,7 @@
   <dimension ref="B3:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2875,7 +2891,7 @@
       <c r="B11" t="s">
         <v>73</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <f>Overview!D21/'Butt Weld'!C10</f>
         <v>1.6592810002229006</v>
       </c>

</xml_diff>